<commit_message>
V1.0 _ ready for EVA
</commit_message>
<xml_diff>
--- a/VI/VI_Modul_Diab.xlsx
+++ b/VI/VI_Modul_Diab.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\filing\doku\HA\Projekte\GiC\Indikatoren\Module\1_Diabetes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HellwigP\Documents\4 Technology\00 Development\VI_generator\VI\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-2146" yWindow="611" windowWidth="13042" windowHeight="5583" tabRatio="880"/>
+    <workbookView xWindow="-1215" yWindow="615" windowWidth="13035" windowHeight="5580" tabRatio="880"/>
   </bookViews>
   <sheets>
     <sheet name="VI_Diab" sheetId="6" r:id="rId1"/>
@@ -7045,27 +7045,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -7098,6 +7077,27 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -8464,44 +8464,44 @@
   <dimension ref="A1:AP99"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="AC34" activePane="bottomRight" state="frozenSplit"/>
       <selection activeCell="C1" sqref="C1"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A46" sqref="A46"/>
-      <selection pane="bottomRight" activeCell="D21" sqref="D21"/>
+      <selection pane="bottomRight" activeCell="AI37" sqref="AI37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2" style="203" customWidth="1"/>
-    <col min="2" max="2" width="8.25" style="4" customWidth="1"/>
-    <col min="3" max="3" width="9.625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="10.25" style="7" customWidth="1"/>
-    <col min="5" max="5" width="22.875" style="7" customWidth="1"/>
-    <col min="6" max="6" width="22.875" style="7" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="39.375" style="3" customWidth="1"/>
-    <col min="8" max="8" width="36.625" style="3" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="16.375" style="4" customWidth="1"/>
-    <col min="10" max="10" width="8.25" style="4" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="10.75" style="4" customWidth="1"/>
-    <col min="12" max="12" width="9.75" style="4" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="8.75" style="156" customWidth="1"/>
-    <col min="14" max="14" width="6.75" style="156" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="6.75" style="156" customWidth="1"/>
-    <col min="16" max="16" width="6.75" style="156" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="7" customWidth="1"/>
+    <col min="5" max="5" width="22.85546875" style="7" customWidth="1"/>
+    <col min="6" max="6" width="22.85546875" style="7" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="39.42578125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="36.5703125" style="3" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="16.42578125" style="4" customWidth="1"/>
+    <col min="10" max="10" width="8.28515625" style="4" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" style="4" customWidth="1"/>
+    <col min="12" max="12" width="9.7109375" style="4" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="8.7109375" style="156" customWidth="1"/>
+    <col min="14" max="14" width="6.7109375" style="156" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="6.7109375" style="156" customWidth="1"/>
+    <col min="16" max="16" width="6.7109375" style="156" hidden="1" customWidth="1"/>
     <col min="17" max="17" width="31" style="7" customWidth="1"/>
-    <col min="18" max="18" width="31.625" style="7" hidden="1" customWidth="1"/>
-    <col min="19" max="20" width="9.5" style="7" customWidth="1"/>
-    <col min="21" max="22" width="10.75" style="7" customWidth="1"/>
-    <col min="23" max="23" width="33.875" style="7" customWidth="1"/>
-    <col min="24" max="24" width="33.875" style="7" hidden="1" customWidth="1"/>
-    <col min="25" max="26" width="10.375" style="7" customWidth="1"/>
-    <col min="27" max="28" width="11.75" style="7" customWidth="1"/>
-    <col min="29" max="33" width="12.5" style="156" customWidth="1"/>
-    <col min="34" max="34" width="14.125" style="2" customWidth="1"/>
-    <col min="35" max="35" width="26.5" style="3" customWidth="1"/>
-    <col min="36" max="36" width="18.125" style="2" customWidth="1"/>
-    <col min="37" max="16384" width="11.5" style="2"/>
+    <col min="18" max="18" width="31.5703125" style="7" hidden="1" customWidth="1"/>
+    <col min="19" max="20" width="9.42578125" style="7" customWidth="1"/>
+    <col min="21" max="22" width="10.7109375" style="7" customWidth="1"/>
+    <col min="23" max="23" width="33.85546875" style="7" customWidth="1"/>
+    <col min="24" max="24" width="33.85546875" style="7" hidden="1" customWidth="1"/>
+    <col min="25" max="26" width="10.42578125" style="7" customWidth="1"/>
+    <col min="27" max="28" width="11.7109375" style="7" customWidth="1"/>
+    <col min="29" max="33" width="12.42578125" style="156" customWidth="1"/>
+    <col min="34" max="34" width="14.140625" style="2" customWidth="1"/>
+    <col min="35" max="35" width="26.42578125" style="3" customWidth="1"/>
+    <col min="36" max="36" width="18.140625" style="2" customWidth="1"/>
+    <col min="37" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:42" ht="59.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -8611,7 +8611,7 @@
         <v>1418</v>
       </c>
     </row>
-    <row r="2" spans="1:42" s="206" customFormat="1" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:42" s="206" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="205"/>
       <c r="B2" s="156">
         <v>0</v>
@@ -8676,7 +8676,7 @@
         <v>1319</v>
       </c>
     </row>
-    <row r="3" spans="1:42" s="11" customFormat="1" ht="42.8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:42" s="11" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="203"/>
       <c r="B3" s="175">
         <v>1</v>
@@ -8780,7 +8780,7 @@
       </c>
       <c r="AJ3" s="2"/>
     </row>
-    <row r="4" spans="1:42" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:42" ht="30" x14ac:dyDescent="0.25">
       <c r="B4" s="175">
         <v>2</v>
       </c>
@@ -8885,7 +8885,7 @@
         <v>1244</v>
       </c>
     </row>
-    <row r="5" spans="1:42" ht="57.1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:42" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="309"/>
       <c r="B5" s="175">
         <v>3</v>
@@ -8989,7 +8989,7 @@
         <v>1243</v>
       </c>
     </row>
-    <row r="6" spans="1:42" ht="42.8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:42" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="309"/>
       <c r="B6" s="175">
         <v>4</v>
@@ -9093,7 +9093,7 @@
         <v>1573</v>
       </c>
     </row>
-    <row r="7" spans="1:42" ht="42.8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:42" ht="45" x14ac:dyDescent="0.25">
       <c r="B7" s="175">
         <v>5</v>
       </c>
@@ -9303,7 +9303,7 @@
         <v>1572</v>
       </c>
     </row>
-    <row r="9" spans="1:42" ht="42.8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:42" ht="60" x14ac:dyDescent="0.25">
       <c r="B9" s="175">
         <v>7</v>
       </c>
@@ -9405,7 +9405,7 @@
         <v>1588</v>
       </c>
     </row>
-    <row r="10" spans="1:42" ht="42.8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:42" ht="45" x14ac:dyDescent="0.25">
       <c r="B10" s="175">
         <v>8</v>
       </c>
@@ -9507,7 +9507,7 @@
         <v>1588</v>
       </c>
     </row>
-    <row r="11" spans="1:42" ht="64.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:42" ht="64.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="175">
         <v>9</v>
       </c>
@@ -9609,7 +9609,7 @@
         <v>1588</v>
       </c>
     </row>
-    <row r="12" spans="1:42" ht="57.1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:42" ht="75" x14ac:dyDescent="0.25">
       <c r="B12" s="175">
         <v>11</v>
       </c>
@@ -9813,7 +9813,7 @@
         <v>1293</v>
       </c>
     </row>
-    <row r="14" spans="1:42" ht="93.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:42" ht="93.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="175">
         <v>13</v>
       </c>
@@ -9915,7 +9915,7 @@
         <v>1317</v>
       </c>
     </row>
-    <row r="15" spans="1:42" ht="57.1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:42" ht="60" x14ac:dyDescent="0.25">
       <c r="B15" s="175">
         <v>14</v>
       </c>
@@ -10017,7 +10017,7 @@
         <v>1293</v>
       </c>
     </row>
-    <row r="16" spans="1:42" ht="42.8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:42" ht="45" x14ac:dyDescent="0.25">
       <c r="B16" s="175">
         <v>15</v>
       </c>
@@ -10119,7 +10119,7 @@
         <v>1293</v>
       </c>
     </row>
-    <row r="17" spans="2:36" ht="42.8" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:36" ht="45" x14ac:dyDescent="0.25">
       <c r="B17" s="175">
         <v>16</v>
       </c>
@@ -10221,7 +10221,7 @@
         <v>1293</v>
       </c>
     </row>
-    <row r="18" spans="2:36" ht="42.8" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:36" ht="60" x14ac:dyDescent="0.25">
       <c r="B18" s="175">
         <v>17</v>
       </c>
@@ -10323,7 +10323,7 @@
         <v>1293</v>
       </c>
     </row>
-    <row r="19" spans="2:36" ht="41.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:36" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="175">
         <v>18</v>
       </c>
@@ -10425,7 +10425,7 @@
         <v>1293</v>
       </c>
     </row>
-    <row r="20" spans="2:36" ht="41.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:36" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="175">
         <v>19</v>
       </c>
@@ -10503,7 +10503,7 @@
       </c>
       <c r="AI20" s="181"/>
     </row>
-    <row r="21" spans="2:36" ht="53.35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:36" ht="53.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="175">
         <v>20</v>
       </c>
@@ -10606,7 +10606,7 @@
       </c>
       <c r="AJ21" s="11"/>
     </row>
-    <row r="22" spans="2:36" ht="44.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:36" ht="44.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="180">
         <v>21</v>
       </c>
@@ -10703,7 +10703,7 @@
       </c>
       <c r="AJ22" s="11"/>
     </row>
-    <row r="23" spans="2:36" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:36" ht="30" x14ac:dyDescent="0.25">
       <c r="B23" s="175">
         <v>22</v>
       </c>
@@ -10805,7 +10805,7 @@
         <v>1317</v>
       </c>
     </row>
-    <row r="24" spans="2:36" ht="42.8" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:36" ht="45" x14ac:dyDescent="0.25">
       <c r="B24" s="175">
         <v>23</v>
       </c>
@@ -10905,7 +10905,7 @@
         <v>1293</v>
       </c>
     </row>
-    <row r="25" spans="2:36" ht="42.8" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:36" ht="45" x14ac:dyDescent="0.25">
       <c r="B25" s="175">
         <v>24</v>
       </c>
@@ -11005,7 +11005,7 @@
         <v>1293</v>
       </c>
     </row>
-    <row r="26" spans="2:36" ht="42.8" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:36" ht="45" x14ac:dyDescent="0.25">
       <c r="B26" s="175">
         <v>25</v>
       </c>
@@ -11105,7 +11105,7 @@
         <v>1293</v>
       </c>
     </row>
-    <row r="27" spans="2:36" ht="42.8" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:36" ht="45" x14ac:dyDescent="0.25">
       <c r="B27" s="175">
         <v>26</v>
       </c>
@@ -11205,7 +11205,7 @@
         <v>1293</v>
       </c>
     </row>
-    <row r="28" spans="2:36" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:36" ht="30" x14ac:dyDescent="0.25">
       <c r="B28" s="175">
         <v>27</v>
       </c>
@@ -11305,7 +11305,7 @@
         <v>1293</v>
       </c>
     </row>
-    <row r="29" spans="2:36" ht="42.8" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:36" ht="45" x14ac:dyDescent="0.25">
       <c r="B29" s="175">
         <v>28</v>
       </c>
@@ -11405,7 +11405,7 @@
         <v>1293</v>
       </c>
     </row>
-    <row r="30" spans="2:36" ht="57.1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:36" ht="75" x14ac:dyDescent="0.25">
       <c r="B30" s="175">
         <v>29</v>
       </c>
@@ -11605,7 +11605,7 @@
         <v>1293</v>
       </c>
     </row>
-    <row r="32" spans="2:36" ht="42.8" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:36" ht="45" x14ac:dyDescent="0.25">
       <c r="B32" s="175">
         <v>31</v>
       </c>
@@ -11705,7 +11705,7 @@
         <v>1293</v>
       </c>
     </row>
-    <row r="33" spans="2:35" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:35" ht="30" x14ac:dyDescent="0.25">
       <c r="B33" s="175">
         <v>32</v>
       </c>
@@ -11805,7 +11805,7 @@
         <v>1325</v>
       </c>
     </row>
-    <row r="34" spans="2:35" ht="42.8" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:35" ht="45" x14ac:dyDescent="0.25">
       <c r="B34" s="175">
         <v>33</v>
       </c>
@@ -11905,7 +11905,7 @@
         <v>1293</v>
       </c>
     </row>
-    <row r="35" spans="2:35" ht="47.55" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:35" ht="47.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="175">
         <v>34</v>
       </c>
@@ -12002,7 +12002,7 @@
         <v>1608</v>
       </c>
     </row>
-    <row r="36" spans="2:35" ht="47.55" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:35" ht="47.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="175">
         <v>35</v>
       </c>
@@ -12100,7 +12100,7 @@
       </c>
       <c r="AI36" s="181"/>
     </row>
-    <row r="37" spans="2:35" ht="47.55" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:35" ht="47.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="175">
         <v>36</v>
       </c>
@@ -12176,13 +12176,13 @@
       <c r="AF37" s="175"/>
       <c r="AG37" s="175"/>
       <c r="AH37" s="190" t="s">
-        <v>1244</v>
+        <v>1319</v>
       </c>
       <c r="AI37" s="181" t="s">
         <v>1743</v>
       </c>
     </row>
-    <row r="38" spans="2:35" ht="48.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:35" ht="48.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="175">
         <v>40</v>
       </c>
@@ -12280,7 +12280,7 @@
       </c>
       <c r="AI38" s="181"/>
     </row>
-    <row r="39" spans="2:35" ht="47.55" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:35" ht="47.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="175">
         <v>41</v>
       </c>
@@ -12380,7 +12380,7 @@
         <v>1293</v>
       </c>
     </row>
-    <row r="40" spans="2:35" ht="42.8" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:35" ht="60" x14ac:dyDescent="0.25">
       <c r="B40" s="175">
         <v>42</v>
       </c>
@@ -12480,7 +12480,7 @@
         <v>1293</v>
       </c>
     </row>
-    <row r="41" spans="2:35" ht="42.8" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:35" ht="60" x14ac:dyDescent="0.25">
       <c r="B41" s="175">
         <v>43</v>
       </c>
@@ -12580,7 +12580,7 @@
         <v>1293</v>
       </c>
     </row>
-    <row r="42" spans="2:35" ht="49.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:35" ht="49.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="175">
         <v>44</v>
       </c>
@@ -12680,7 +12680,7 @@
         <v>1293</v>
       </c>
     </row>
-    <row r="43" spans="2:35" ht="42.8" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:35" ht="45" x14ac:dyDescent="0.25">
       <c r="B43" s="175">
         <v>45</v>
       </c>
@@ -12780,7 +12780,7 @@
         <v>1293</v>
       </c>
     </row>
-    <row r="44" spans="2:35" ht="42.8" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:35" ht="45" x14ac:dyDescent="0.25">
       <c r="B44" s="175">
         <v>46</v>
       </c>
@@ -12878,7 +12878,7 @@
       </c>
       <c r="AI44" s="181"/>
     </row>
-    <row r="45" spans="2:35" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:35" ht="45" x14ac:dyDescent="0.25">
       <c r="B45" s="175">
         <v>47</v>
       </c>
@@ -12956,7 +12956,7 @@
       </c>
       <c r="AI45" s="181"/>
     </row>
-    <row r="46" spans="2:35" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:35" ht="45" x14ac:dyDescent="0.25">
       <c r="B46" s="175">
         <v>50</v>
       </c>
@@ -13056,7 +13056,7 @@
         <v>1547</v>
       </c>
     </row>
-    <row r="47" spans="2:35" ht="48.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:35" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="175">
         <v>51</v>
       </c>
@@ -13356,7 +13356,7 @@
         <v>1331</v>
       </c>
     </row>
-    <row r="50" spans="2:35" ht="50.3" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:35" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="175">
         <v>54</v>
       </c>
@@ -13456,7 +13456,7 @@
         <v>1331</v>
       </c>
     </row>
-    <row r="51" spans="2:35" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:35" ht="45" x14ac:dyDescent="0.25">
       <c r="B51" s="175">
         <v>55</v>
       </c>
@@ -13556,7 +13556,7 @@
         <v>1331</v>
       </c>
     </row>
-    <row r="52" spans="2:35" ht="45.55" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:35" ht="45.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="175">
         <v>56</v>
       </c>
@@ -13656,7 +13656,7 @@
         <v>1331</v>
       </c>
     </row>
-    <row r="53" spans="2:35" ht="42.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:35" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="175">
         <v>57</v>
       </c>
@@ -13856,7 +13856,7 @@
         <v>1331</v>
       </c>
     </row>
-    <row r="55" spans="2:35" ht="44.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:35" ht="44.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" s="175">
         <v>59</v>
       </c>
@@ -13956,7 +13956,7 @@
         <v>1293</v>
       </c>
     </row>
-    <row r="56" spans="2:35" ht="42.8" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:35" ht="45" x14ac:dyDescent="0.25">
       <c r="B56" s="175">
         <v>60</v>
       </c>
@@ -14056,7 +14056,7 @@
         <v>1293</v>
       </c>
     </row>
-    <row r="57" spans="2:35" ht="42.8" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:35" ht="45" x14ac:dyDescent="0.25">
       <c r="B57" s="175">
         <v>61</v>
       </c>
@@ -14156,7 +14156,7 @@
         <v>1293</v>
       </c>
     </row>
-    <row r="58" spans="2:35" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:35" ht="45" x14ac:dyDescent="0.25">
       <c r="B58" s="175">
         <v>62</v>
       </c>
@@ -14256,7 +14256,7 @@
         <v>1293</v>
       </c>
     </row>
-    <row r="59" spans="2:35" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:35" ht="45" x14ac:dyDescent="0.25">
       <c r="B59" s="175">
         <v>63</v>
       </c>
@@ -14356,7 +14356,7 @@
         <v>1293</v>
       </c>
     </row>
-    <row r="60" spans="2:35" ht="42.8" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:35" ht="45" x14ac:dyDescent="0.25">
       <c r="B60" s="175">
         <v>64</v>
       </c>
@@ -14456,7 +14456,7 @@
         <v>1293</v>
       </c>
     </row>
-    <row r="61" spans="2:35" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:35" ht="45" x14ac:dyDescent="0.25">
       <c r="B61" s="175">
         <v>65</v>
       </c>
@@ -14556,7 +14556,7 @@
         <v>1293</v>
       </c>
     </row>
-    <row r="62" spans="2:35" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:35" ht="45" x14ac:dyDescent="0.25">
       <c r="B62" s="175">
         <v>66</v>
       </c>
@@ -14656,7 +14656,7 @@
         <v>1293</v>
       </c>
     </row>
-    <row r="63" spans="2:35" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:35" ht="30" x14ac:dyDescent="0.25">
       <c r="B63" s="175">
         <v>67</v>
       </c>
@@ -14756,7 +14756,7 @@
         <v>1293</v>
       </c>
     </row>
-    <row r="64" spans="2:35" ht="42.8" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:35" ht="45" x14ac:dyDescent="0.25">
       <c r="B64" s="175">
         <v>68</v>
       </c>
@@ -14856,7 +14856,7 @@
         <v>1293</v>
       </c>
     </row>
-    <row r="65" spans="2:35" ht="42.8" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:35" ht="45" x14ac:dyDescent="0.25">
       <c r="B65" s="175">
         <v>69</v>
       </c>
@@ -14956,7 +14956,7 @@
         <v>1293</v>
       </c>
     </row>
-    <row r="66" spans="2:35" ht="43.85" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:35" ht="43.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B66" s="175">
         <v>70</v>
       </c>
@@ -15056,7 +15056,7 @@
         <v>1331</v>
       </c>
     </row>
-    <row r="67" spans="2:35" ht="40.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:35" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B67" s="175">
         <v>71</v>
       </c>
@@ -15156,7 +15156,7 @@
         <v>1331</v>
       </c>
     </row>
-    <row r="68" spans="2:35" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:35" ht="30" x14ac:dyDescent="0.25">
       <c r="B68" s="175">
         <v>72</v>
       </c>
@@ -15256,7 +15256,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="69" spans="2:35" ht="42.8" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:35" ht="60" x14ac:dyDescent="0.25">
       <c r="B69" s="175">
         <v>80</v>
       </c>
@@ -15356,7 +15356,7 @@
         <v>1293</v>
       </c>
     </row>
-    <row r="70" spans="2:35" ht="40.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:35" ht="40.700000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B70" s="175">
         <v>81</v>
       </c>
@@ -15456,7 +15456,7 @@
         <v>1293</v>
       </c>
     </row>
-    <row r="71" spans="2:35" ht="57.1" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:35" ht="60" x14ac:dyDescent="0.25">
       <c r="B71" s="175">
         <v>82</v>
       </c>
@@ -15556,7 +15556,7 @@
         <v>1293</v>
       </c>
     </row>
-    <row r="72" spans="2:35" ht="42.8" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:35" ht="45" x14ac:dyDescent="0.25">
       <c r="B72" s="175">
         <v>83</v>
       </c>
@@ -15656,7 +15656,7 @@
         <v>1293</v>
       </c>
     </row>
-    <row r="73" spans="2:35" ht="71.349999999999994" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:35" ht="75" x14ac:dyDescent="0.25">
       <c r="B73" s="175">
         <v>84</v>
       </c>
@@ -15756,7 +15756,7 @@
         <v>1331</v>
       </c>
     </row>
-    <row r="74" spans="2:35" ht="57.1" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:35" ht="60" x14ac:dyDescent="0.25">
       <c r="B74" s="175">
         <v>85</v>
       </c>
@@ -15856,7 +15856,7 @@
         <v>1293</v>
       </c>
     </row>
-    <row r="75" spans="2:35" ht="42.8" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:35" ht="60" x14ac:dyDescent="0.25">
       <c r="B75" s="175">
         <v>86</v>
       </c>
@@ -15956,7 +15956,7 @@
         <v>1293</v>
       </c>
     </row>
-    <row r="76" spans="2:35" ht="80.349999999999994" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:35" ht="80.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B76" s="175">
         <v>87</v>
       </c>
@@ -16056,7 +16056,7 @@
         <v>1293</v>
       </c>
     </row>
-    <row r="77" spans="2:35" ht="47.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:35" ht="47.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B77" s="175">
         <v>88</v>
       </c>
@@ -16156,7 +16156,7 @@
         <v>1545</v>
       </c>
     </row>
-    <row r="78" spans="2:35" ht="42.8" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:35" ht="45" x14ac:dyDescent="0.25">
       <c r="B78" s="175">
         <v>89</v>
       </c>
@@ -16256,7 +16256,7 @@
         <v>1546</v>
       </c>
     </row>
-    <row r="79" spans="2:35" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:35" ht="45" x14ac:dyDescent="0.25">
       <c r="B79" s="175">
         <v>90</v>
       </c>
@@ -16356,7 +16356,7 @@
         <v>1337</v>
       </c>
     </row>
-    <row r="80" spans="2:35" ht="42.8" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:35" ht="45" x14ac:dyDescent="0.25">
       <c r="B80" s="175">
         <v>91</v>
       </c>
@@ -16456,7 +16456,7 @@
         <v>1337</v>
       </c>
     </row>
-    <row r="81" spans="2:35" ht="42.8" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:35" ht="60" x14ac:dyDescent="0.25">
       <c r="B81" s="175">
         <v>92</v>
       </c>
@@ -16556,7 +16556,7 @@
         <v>1293</v>
       </c>
     </row>
-    <row r="82" spans="2:35" ht="42.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:35" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B82" s="175">
         <v>93</v>
       </c>
@@ -16656,7 +16656,7 @@
         <v>1298</v>
       </c>
     </row>
-    <row r="83" spans="2:35" ht="42.8" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:35" ht="45" x14ac:dyDescent="0.25">
       <c r="B83" s="175">
         <v>94</v>
       </c>
@@ -16756,7 +16756,7 @@
         <v>1293</v>
       </c>
     </row>
-    <row r="84" spans="2:35" ht="42.8" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:35" ht="45" x14ac:dyDescent="0.25">
       <c r="B84" s="175">
         <v>95</v>
       </c>
@@ -16856,7 +16856,7 @@
         <v>1293</v>
       </c>
     </row>
-    <row r="85" spans="2:35" ht="42.8" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:35" ht="45" x14ac:dyDescent="0.25">
       <c r="B85" s="175">
         <v>96</v>
       </c>
@@ -16956,7 +16956,7 @@
         <v>1325</v>
       </c>
     </row>
-    <row r="86" spans="2:35" ht="49.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:35" ht="49.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B86" s="175">
         <v>97</v>
       </c>
@@ -17056,7 +17056,7 @@
         <v>1302</v>
       </c>
     </row>
-    <row r="87" spans="2:35" ht="42.8" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:35" ht="45" x14ac:dyDescent="0.25">
       <c r="B87" s="175">
         <v>100</v>
       </c>
@@ -17156,7 +17156,7 @@
         <v>1301</v>
       </c>
     </row>
-    <row r="88" spans="2:35" ht="42.8" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:35" ht="45" x14ac:dyDescent="0.25">
       <c r="B88" s="175">
         <v>101</v>
       </c>
@@ -17256,7 +17256,7 @@
         <v>1301</v>
       </c>
     </row>
-    <row r="89" spans="2:35" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:35" ht="45" x14ac:dyDescent="0.25">
       <c r="B89" s="175">
         <v>102</v>
       </c>
@@ -17356,7 +17356,7 @@
         <v>1301</v>
       </c>
     </row>
-    <row r="90" spans="2:35" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:35" ht="30" x14ac:dyDescent="0.25">
       <c r="B90" s="175">
         <v>103</v>
       </c>
@@ -17456,7 +17456,7 @@
         <v>1301</v>
       </c>
     </row>
-    <row r="91" spans="2:35" ht="30.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:35" ht="30.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C91" s="37"/>
       <c r="D91" s="2"/>
       <c r="E91" s="18"/>
@@ -17791,48 +17791,48 @@
       <selection activeCell="J39" sqref="J39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="2.625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="18.5" style="2" customWidth="1"/>
-    <col min="4" max="4" width="10.25" style="2" customWidth="1"/>
-    <col min="5" max="7" width="10.75" style="2" customWidth="1"/>
-    <col min="8" max="8" width="21.875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="12.625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="9.625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="10.125" style="2" customWidth="1"/>
-    <col min="12" max="12" width="7.875" style="2" customWidth="1"/>
-    <col min="13" max="13" width="7.5" style="2" customWidth="1"/>
-    <col min="14" max="14" width="8.5" style="2" customWidth="1"/>
-    <col min="15" max="15" width="13.625" style="2" customWidth="1"/>
-    <col min="16" max="16" width="7.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="6.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="6.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="6.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="7.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="25" max="16384" width="11.5" style="2"/>
+    <col min="1" max="1" width="1.5703125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="2.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="2" customWidth="1"/>
+    <col min="5" max="7" width="10.7109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="21.85546875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="9.5703125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="10.140625" style="2" customWidth="1"/>
+    <col min="12" max="12" width="7.85546875" style="2" customWidth="1"/>
+    <col min="13" max="13" width="7.42578125" style="2" customWidth="1"/>
+    <col min="14" max="14" width="8.42578125" style="2" customWidth="1"/>
+    <col min="15" max="15" width="13.5703125" style="2" customWidth="1"/>
+    <col min="16" max="16" width="7.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="8.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="25" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:38" ht="8.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:38" ht="14.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:38" ht="8.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:38" ht="14.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C2" s="27" t="s">
         <v>1250</v>
       </c>
       <c r="L2" s="76"/>
     </row>
-    <row r="3" spans="2:38" ht="15.65" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:38" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C3" s="38" t="s">
         <v>1131</v>
       </c>
-      <c r="D3" s="344">
+      <c r="D3" s="337">
         <v>41697</v>
       </c>
-      <c r="E3" s="344"/>
+      <c r="E3" s="337"/>
       <c r="F3" s="61"/>
       <c r="G3" s="61"/>
       <c r="H3" s="61"/>
@@ -17843,30 +17843,30 @@
       <c r="M3" s="61"/>
       <c r="N3" s="61"/>
     </row>
-    <row r="4" spans="2:38" ht="15.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:38" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L4" s="38"/>
       <c r="M4" s="38"/>
       <c r="N4" s="38"/>
       <c r="O4" s="38"/>
-      <c r="AG4" s="337" t="s">
+      <c r="AG4" s="349" t="s">
         <v>1129</v>
       </c>
-      <c r="AH4" s="337"/>
-      <c r="AI4" s="337"/>
-      <c r="AJ4" s="337"/>
-      <c r="AK4" s="337"/>
-      <c r="AL4" s="337"/>
-    </row>
-    <row r="5" spans="2:38" x14ac:dyDescent="0.25">
+      <c r="AH4" s="349"/>
+      <c r="AI4" s="349"/>
+      <c r="AJ4" s="349"/>
+      <c r="AK4" s="349"/>
+      <c r="AL4" s="349"/>
+    </row>
+    <row r="5" spans="2:38" ht="14.25" x14ac:dyDescent="0.25">
       <c r="C5" s="8" t="s">
         <v>1132</v>
       </c>
     </row>
-    <row r="6" spans="2:38" ht="49.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="348" t="s">
+    <row r="6" spans="2:38" ht="49.7" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="341" t="s">
         <v>1253</v>
       </c>
-      <c r="D6" s="349"/>
+      <c r="D6" s="342"/>
       <c r="E6" s="40" t="s">
         <v>1266</v>
       </c>
@@ -17877,12 +17877,12 @@
         <v>1268</v>
       </c>
     </row>
-    <row r="7" spans="2:38" ht="16.3" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:38" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="8"/>
-      <c r="C7" s="350" t="s">
+      <c r="C7" s="343" t="s">
         <v>1252</v>
       </c>
-      <c r="D7" s="350"/>
+      <c r="D7" s="343"/>
       <c r="E7" s="152">
         <v>0.99</v>
       </c>
@@ -17894,15 +17894,15 @@
         <v>9.000000000000008E-2</v>
       </c>
       <c r="H7" s="121"/>
-      <c r="I7" s="343"/>
-      <c r="J7" s="343"/>
-    </row>
-    <row r="8" spans="2:38" ht="15.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I7" s="336"/>
+      <c r="J7" s="336"/>
+    </row>
+    <row r="8" spans="2:38" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="8"/>
-      <c r="C8" s="350" t="s">
+      <c r="C8" s="343" t="s">
         <v>1126</v>
       </c>
-      <c r="D8" s="350"/>
+      <c r="D8" s="343"/>
       <c r="E8" s="152">
         <v>0.99</v>
       </c>
@@ -17914,15 +17914,15 @@
         <v>2.0000000000000018E-2</v>
       </c>
       <c r="H8" s="121"/>
-      <c r="I8" s="339"/>
-      <c r="J8" s="339"/>
+      <c r="I8" s="346"/>
+      <c r="J8" s="346"/>
     </row>
     <row r="9" spans="2:38" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="8"/>
-      <c r="C9" s="350" t="s">
+      <c r="C9" s="343" t="s">
         <v>1303</v>
       </c>
-      <c r="D9" s="350"/>
+      <c r="D9" s="343"/>
       <c r="E9" s="152">
         <v>1.01</v>
       </c>
@@ -17945,10 +17945,10 @@
     </row>
     <row r="10" spans="2:38" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="8"/>
-      <c r="C10" s="350" t="s">
+      <c r="C10" s="343" t="s">
         <v>1127</v>
       </c>
-      <c r="D10" s="350"/>
+      <c r="D10" s="343"/>
       <c r="E10" s="152">
         <v>1</v>
       </c>
@@ -17971,10 +17971,10 @@
     </row>
     <row r="11" spans="2:38" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="8"/>
-      <c r="C11" s="351" t="s">
+      <c r="C11" s="344" t="s">
         <v>1133</v>
       </c>
-      <c r="D11" s="351"/>
+      <c r="D11" s="344"/>
       <c r="E11" s="153">
         <f>SUM(E7:E10)/4</f>
         <v>0.99750000000000005</v>
@@ -18013,12 +18013,12 @@
       <c r="O12" s="20"/>
       <c r="P12" s="20"/>
     </row>
-    <row r="13" spans="2:38" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:38" ht="14.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="C13" s="8" t="s">
         <v>1134</v>
       </c>
     </row>
-    <row r="14" spans="2:38" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:38" ht="14.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="B14" s="8"/>
       <c r="C14" s="67" t="s">
         <v>481</v>
@@ -18038,7 +18038,7 @@
       <c r="N14" s="37"/>
       <c r="O14" s="37"/>
     </row>
-    <row r="15" spans="2:38" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:38" ht="14.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="B15" s="8"/>
       <c r="C15" s="68"/>
       <c r="D15" s="326" t="s">
@@ -18058,29 +18058,29 @@
       <c r="N15" s="37"/>
       <c r="O15" s="37"/>
     </row>
-    <row r="16" spans="2:38" ht="15.15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:38" ht="15.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="8"/>
       <c r="C16" s="68"/>
-      <c r="D16" s="345" t="s">
+      <c r="D16" s="338" t="s">
         <v>1136</v>
       </c>
-      <c r="E16" s="346"/>
-      <c r="F16" s="345" t="s">
+      <c r="E16" s="339"/>
+      <c r="F16" s="338" t="s">
         <v>474</v>
       </c>
-      <c r="G16" s="347"/>
+      <c r="G16" s="340"/>
       <c r="H16" s="326" t="s">
         <v>474</v>
       </c>
       <c r="I16" s="328"/>
       <c r="J16" s="10"/>
       <c r="K16" s="10"/>
-      <c r="L16" s="334"/>
-      <c r="M16" s="334"/>
-      <c r="N16" s="334"/>
-      <c r="O16" s="334"/>
-    </row>
-    <row r="17" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="L16" s="345"/>
+      <c r="M16" s="345"/>
+      <c r="N16" s="345"/>
+      <c r="O16" s="345"/>
+    </row>
+    <row r="17" spans="2:15" ht="14.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="B17" s="8"/>
       <c r="C17" s="71" t="s">
         <v>1130</v>
@@ -18110,7 +18110,7 @@
       <c r="N17" s="9"/>
       <c r="O17" s="9"/>
     </row>
-    <row r="18" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:15" ht="14.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="B18" s="8"/>
       <c r="C18" s="321" t="s">
         <v>475</v>
@@ -18140,7 +18140,7 @@
       <c r="N18" s="73"/>
       <c r="O18" s="25"/>
     </row>
-    <row r="19" spans="2:15" s="81" customFormat="1" ht="11.55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:15" s="81" customFormat="1" ht="11.65" hidden="1" x14ac:dyDescent="0.2">
       <c r="B19" s="79"/>
       <c r="C19" s="322"/>
       <c r="D19" s="104"/>
@@ -18160,7 +18160,7 @@
       <c r="N19" s="85"/>
       <c r="O19" s="82"/>
     </row>
-    <row r="20" spans="2:15" ht="16.3" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:15" ht="16.350000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="8"/>
       <c r="C20" s="86" t="s">
         <v>476</v>
@@ -18190,7 +18190,7 @@
       <c r="N20" s="73"/>
       <c r="O20" s="25"/>
     </row>
-    <row r="21" spans="2:15" s="98" customFormat="1" ht="16.3" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:15" s="98" customFormat="1" ht="16.350000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="94"/>
       <c r="C21" s="90"/>
       <c r="D21" s="104"/>
@@ -18256,7 +18256,7 @@
       <c r="N23" s="88"/>
       <c r="O23" s="97"/>
     </row>
-    <row r="24" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:15" ht="14.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="C24" s="86" t="s">
         <v>478</v>
       </c>
@@ -18284,7 +18284,7 @@
       <c r="N24" s="73"/>
       <c r="O24" s="25"/>
     </row>
-    <row r="25" spans="2:15" s="98" customFormat="1" ht="11.55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:15" s="98" customFormat="1" ht="11.65" hidden="1" x14ac:dyDescent="0.2">
       <c r="C25" s="90"/>
       <c r="D25" s="104"/>
       <c r="E25" s="104"/>
@@ -18302,7 +18302,7 @@
       <c r="N25" s="88"/>
       <c r="O25" s="97"/>
     </row>
-    <row r="26" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:15" ht="14.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="C26" s="67" t="s">
         <v>479</v>
       </c>
@@ -18330,7 +18330,7 @@
       <c r="N26" s="73"/>
       <c r="O26" s="25"/>
     </row>
-    <row r="27" spans="2:15" s="98" customFormat="1" ht="11.55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:15" s="98" customFormat="1" ht="11.65" hidden="1" x14ac:dyDescent="0.2">
       <c r="C27" s="90"/>
       <c r="D27" s="104"/>
       <c r="E27" s="104"/>
@@ -18348,7 +18348,7 @@
       <c r="N27" s="88"/>
       <c r="O27" s="97"/>
     </row>
-    <row r="28" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:15" ht="14.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="C28" s="111" t="s">
         <v>480</v>
       </c>
@@ -18376,7 +18376,7 @@
       <c r="N28" s="75"/>
       <c r="O28" s="26"/>
     </row>
-    <row r="29" spans="2:15" s="98" customFormat="1" ht="11.55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:15" s="98" customFormat="1" ht="11.65" hidden="1" x14ac:dyDescent="0.2">
       <c r="C29" s="99"/>
       <c r="D29" s="106"/>
       <c r="E29" s="106"/>
@@ -18394,12 +18394,12 @@
       <c r="N29" s="102"/>
       <c r="O29" s="101"/>
     </row>
-    <row r="30" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:15" ht="14.25" x14ac:dyDescent="0.25">
       <c r="C30" s="157"/>
       <c r="D30" s="30"/>
-      <c r="E30" s="334"/>
-      <c r="F30" s="334"/>
-      <c r="G30" s="334"/>
+      <c r="E30" s="345"/>
+      <c r="F30" s="345"/>
+      <c r="G30" s="345"/>
       <c r="H30" s="62"/>
       <c r="I30" s="37"/>
       <c r="J30" s="37" t="s">
@@ -18407,11 +18407,11 @@
       </c>
       <c r="K30" s="37"/>
       <c r="L30" s="62"/>
-      <c r="M30" s="334"/>
-      <c r="N30" s="334"/>
-      <c r="O30" s="334"/>
-    </row>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="M30" s="345"/>
+      <c r="N30" s="345"/>
+      <c r="O30" s="345"/>
+    </row>
+    <row r="31" spans="2:15" ht="14.25" x14ac:dyDescent="0.25">
       <c r="C31" s="20"/>
       <c r="D31" s="20"/>
       <c r="E31" s="20"/>
@@ -18438,12 +18438,12 @@
         <v>1272</v>
       </c>
       <c r="J32" s="64"/>
-      <c r="K32" s="340"/>
-      <c r="L32" s="340"/>
-      <c r="M32" s="338"/>
-      <c r="N32" s="338"/>
-    </row>
-    <row r="33" spans="3:15" ht="47.55" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K32" s="351"/>
+      <c r="L32" s="351"/>
+      <c r="M32" s="350"/>
+      <c r="N32" s="350"/>
+    </row>
+    <row r="33" spans="3:15" ht="47.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C33" s="159" t="s">
         <v>1278</v>
       </c>
@@ -18469,7 +18469,7 @@
       <c r="M33" s="20"/>
       <c r="N33" s="20"/>
     </row>
-    <row r="34" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:15" ht="14.25" x14ac:dyDescent="0.25">
       <c r="C34" s="162" t="s">
         <v>1270</v>
       </c>
@@ -18499,7 +18499,7 @@
       <c r="N34" s="125"/>
       <c r="O34" s="20"/>
     </row>
-    <row r="35" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:15" ht="14.25" x14ac:dyDescent="0.25">
       <c r="C35" s="135" t="s">
         <v>1271</v>
       </c>
@@ -18529,7 +18529,7 @@
       <c r="N35" s="125"/>
       <c r="O35" s="20"/>
     </row>
-    <row r="36" spans="3:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:15" ht="14.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="C36" s="130">
         <v>2012</v>
       </c>
@@ -18553,7 +18553,7 @@
       <c r="M36" s="120"/>
       <c r="N36" s="128"/>
     </row>
-    <row r="37" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:15" ht="14.25" x14ac:dyDescent="0.25">
       <c r="D37" s="139"/>
       <c r="E37" s="139"/>
       <c r="F37" s="140">
@@ -18564,10 +18564,10 @@
       <c r="H37" s="141"/>
       <c r="I37" s="20"/>
       <c r="J37" s="25"/>
-      <c r="K37" s="339"/>
-      <c r="L37" s="339"/>
-      <c r="M37" s="334"/>
-      <c r="N37" s="334"/>
+      <c r="K37" s="346"/>
+      <c r="L37" s="346"/>
+      <c r="M37" s="345"/>
+      <c r="N37" s="345"/>
     </row>
     <row r="38" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C38" s="66" t="s">
@@ -18583,10 +18583,10 @@
       <c r="J38" s="25"/>
       <c r="K38" s="143"/>
       <c r="L38" s="143"/>
-      <c r="M38" s="334"/>
-      <c r="N38" s="334"/>
-    </row>
-    <row r="39" spans="3:15" ht="42.8" x14ac:dyDescent="0.25">
+      <c r="M38" s="345"/>
+      <c r="N38" s="345"/>
+    </row>
+    <row r="39" spans="3:15" ht="42.75" x14ac:dyDescent="0.25">
       <c r="C39" s="133" t="s">
         <v>1280</v>
       </c>
@@ -18609,10 +18609,10 @@
       <c r="J39" s="122"/>
       <c r="K39" s="144"/>
       <c r="L39" s="144"/>
-      <c r="M39" s="338"/>
-      <c r="N39" s="338"/>
-    </row>
-    <row r="40" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="M39" s="350"/>
+      <c r="N39" s="350"/>
+    </row>
+    <row r="40" spans="3:15" ht="14.25" x14ac:dyDescent="0.25">
       <c r="C40" s="162" t="s">
         <v>1270</v>
       </c>
@@ -18641,7 +18641,7 @@
       <c r="M40" s="20"/>
       <c r="N40" s="20"/>
     </row>
-    <row r="41" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:15" ht="14.25" x14ac:dyDescent="0.25">
       <c r="C41" s="135" t="s">
         <v>1271</v>
       </c>
@@ -18670,7 +18670,7 @@
       <c r="M41" s="137"/>
       <c r="N41" s="137"/>
     </row>
-    <row r="42" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:15" ht="14.25" x14ac:dyDescent="0.25">
       <c r="C42" s="118"/>
       <c r="D42" s="118"/>
       <c r="E42" s="118"/>
@@ -18698,10 +18698,10 @@
       <c r="J43" s="120"/>
       <c r="K43" s="37"/>
       <c r="L43" s="37"/>
-      <c r="M43" s="334"/>
-      <c r="N43" s="334"/>
-    </row>
-    <row r="44" spans="3:15" ht="42.8" x14ac:dyDescent="0.25">
+      <c r="M43" s="345"/>
+      <c r="N43" s="345"/>
+    </row>
+    <row r="44" spans="3:15" ht="42.75" x14ac:dyDescent="0.25">
       <c r="C44" s="133" t="s">
         <v>1283</v>
       </c>
@@ -18721,7 +18721,7 @@
         <v>1251</v>
       </c>
     </row>
-    <row r="45" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:15" ht="14.25" x14ac:dyDescent="0.25">
       <c r="C45" s="162" t="s">
         <v>1270</v>
       </c>
@@ -18744,7 +18744,7 @@
         <v>1.0153256704980842</v>
       </c>
     </row>
-    <row r="46" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:15" ht="14.25" x14ac:dyDescent="0.25">
       <c r="C46" s="135" t="s">
         <v>1271</v>
       </c>
@@ -18767,10 +18767,10 @@
         <v>-3.3844189016602841E-2</v>
       </c>
     </row>
-    <row r="48" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:15" ht="14.25" x14ac:dyDescent="0.25">
       <c r="I48" s="8"/>
     </row>
-    <row r="49" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="4:8" ht="14.25" x14ac:dyDescent="0.25">
       <c r="D49" s="120"/>
       <c r="F49" s="145" t="s">
         <v>1284</v>
@@ -18785,21 +18785,21 @@
         <v>1251</v>
       </c>
     </row>
-    <row r="51" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="F51" s="335" t="s">
+    <row r="51" spans="4:8" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="F51" s="347" t="s">
         <v>1270</v>
       </c>
-      <c r="G51" s="336"/>
+      <c r="G51" s="348"/>
       <c r="H51" s="164">
         <f>(H40+H34+H45)/3</f>
         <v>1.0004587047825326</v>
       </c>
     </row>
-    <row r="52" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="F52" s="341" t="s">
+    <row r="52" spans="4:8" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="F52" s="334" t="s">
         <v>1271</v>
       </c>
-      <c r="G52" s="342"/>
+      <c r="G52" s="335"/>
       <c r="H52" s="165">
         <f>(H41+H35+H46)/3</f>
         <v>3.5746386417047145E-2</v>
@@ -18807,6 +18807,19 @@
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="L16:O16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="AG4:AL4"/>
+    <mergeCell ref="M43:N43"/>
+    <mergeCell ref="M38:N38"/>
+    <mergeCell ref="M39:N39"/>
+    <mergeCell ref="K37:L37"/>
+    <mergeCell ref="M37:N37"/>
+    <mergeCell ref="K32:L32"/>
+    <mergeCell ref="M32:N32"/>
+    <mergeCell ref="M30:O30"/>
     <mergeCell ref="F52:G52"/>
     <mergeCell ref="I7:J7"/>
     <mergeCell ref="D3:E3"/>
@@ -18823,19 +18836,6 @@
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="E30:G30"/>
     <mergeCell ref="I8:J8"/>
-    <mergeCell ref="L16:O16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="F51:G51"/>
-    <mergeCell ref="AG4:AL4"/>
-    <mergeCell ref="M43:N43"/>
-    <mergeCell ref="M38:N38"/>
-    <mergeCell ref="M39:N39"/>
-    <mergeCell ref="K37:L37"/>
-    <mergeCell ref="M37:N37"/>
-    <mergeCell ref="K32:L32"/>
-    <mergeCell ref="M32:N32"/>
-    <mergeCell ref="M30:O30"/>
   </mergeCells>
   <conditionalFormatting sqref="H46 H41 H35">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
@@ -18867,26 +18867,26 @@
       <selection pane="bottomLeft" activeCell="E117" sqref="E117"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.5" style="12" customWidth="1"/>
-    <col min="2" max="2" width="39.125" style="2" customWidth="1"/>
-    <col min="3" max="4" width="11.625" style="13" customWidth="1"/>
-    <col min="5" max="5" width="23.875" style="4" customWidth="1"/>
-    <col min="6" max="6" width="40.75" style="4" customWidth="1"/>
-    <col min="7" max="7" width="17.375" style="3" customWidth="1"/>
-    <col min="8" max="8" width="19.375" style="4" customWidth="1"/>
-    <col min="9" max="9" width="11.5" style="4" customWidth="1"/>
+    <col min="1" max="1" width="2.42578125" style="12" customWidth="1"/>
+    <col min="2" max="2" width="39.140625" style="2" customWidth="1"/>
+    <col min="3" max="4" width="11.5703125" style="13" customWidth="1"/>
+    <col min="5" max="5" width="23.85546875" style="4" customWidth="1"/>
+    <col min="6" max="6" width="40.7109375" style="4" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" style="4" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="4" customWidth="1"/>
     <col min="10" max="10" width="72" style="3" customWidth="1"/>
-    <col min="11" max="11" width="85.375" style="2" customWidth="1"/>
-    <col min="12" max="12" width="46.25" style="2" customWidth="1"/>
-    <col min="13" max="13" width="16.625" style="2" customWidth="1"/>
-    <col min="14" max="14" width="23.375" style="2" customWidth="1"/>
-    <col min="15" max="16384" width="11.5" style="2"/>
+    <col min="11" max="11" width="85.42578125" style="2" customWidth="1"/>
+    <col min="12" max="12" width="46.28515625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="16.5703125" style="2" customWidth="1"/>
+    <col min="14" max="14" width="23.42578125" style="2" customWidth="1"/>
+    <col min="15" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="14.95" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:12" s="3" customFormat="1" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:12" s="3" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="199"/>
       <c r="B2" s="15" t="s">
         <v>207</v>
@@ -18920,7 +18920,7 @@
         <v>1287</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="3" customFormat="1" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="199"/>
       <c r="B3" s="215" t="s">
         <v>912</v>
@@ -18954,7 +18954,7 @@
         <v>1446</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="3" customFormat="1" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" s="3" customFormat="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="199"/>
       <c r="B4" s="223"/>
       <c r="C4" s="209"/>
@@ -18976,7 +18976,7 @@
       <c r="K4" s="228"/>
       <c r="L4" s="228"/>
     </row>
-    <row r="5" spans="1:12" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
       <c r="B5" s="215" t="s">
         <v>1738</v>
       </c>
@@ -19023,7 +19023,7 @@
       <c r="K6" s="232"/>
       <c r="L6" s="232"/>
     </row>
-    <row r="7" spans="1:12" ht="114.15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="114.2" x14ac:dyDescent="0.25">
       <c r="B7" s="233" t="s">
         <v>42</v>
       </c>
@@ -19054,7 +19054,7 @@
       </c>
       <c r="L7" s="228"/>
     </row>
-    <row r="8" spans="1:12" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="237"/>
       <c r="C8" s="177"/>
       <c r="D8" s="177" t="s">
@@ -19071,7 +19071,7 @@
       <c r="K8" s="228"/>
       <c r="L8" s="228"/>
     </row>
-    <row r="9" spans="1:12" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
       <c r="B9" s="233" t="s">
         <v>43</v>
       </c>
@@ -19098,7 +19098,7 @@
       <c r="K9" s="228"/>
       <c r="L9" s="228"/>
     </row>
-    <row r="10" spans="1:12" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="238"/>
       <c r="C10" s="202"/>
       <c r="D10" s="202" t="s">
@@ -19144,7 +19144,7 @@
       <c r="K11" s="228"/>
       <c r="L11" s="228"/>
     </row>
-    <row r="12" spans="1:12" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
       <c r="B12" s="233" t="s">
         <v>1739</v>
       </c>
@@ -19173,7 +19173,7 @@
       <c r="K12" s="228"/>
       <c r="L12" s="228"/>
     </row>
-    <row r="13" spans="1:12" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="237"/>
       <c r="C13" s="177"/>
       <c r="D13" s="177" t="s">
@@ -19190,7 +19190,7 @@
       <c r="K13" s="228"/>
       <c r="L13" s="228"/>
     </row>
-    <row r="14" spans="1:12" ht="57.1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="57.2" x14ac:dyDescent="0.25">
       <c r="B14" s="233" t="s">
         <v>1590</v>
       </c>
@@ -19219,7 +19219,7 @@
       <c r="K14" s="228"/>
       <c r="L14" s="228"/>
     </row>
-    <row r="15" spans="1:12" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="241"/>
       <c r="C15" s="209"/>
       <c r="D15" s="209" t="s">
@@ -19236,7 +19236,7 @@
       <c r="K15" s="228"/>
       <c r="L15" s="228"/>
     </row>
-    <row r="16" spans="1:12" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="238" t="s">
         <v>61</v>
       </c>
@@ -19261,7 +19261,7 @@
       <c r="K16" s="228"/>
       <c r="L16" s="228"/>
     </row>
-    <row r="17" spans="1:13" ht="73.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="73.349999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="233" t="s">
         <v>66</v>
       </c>
@@ -19313,7 +19313,7 @@
       <c r="K18" s="228"/>
       <c r="L18" s="228"/>
     </row>
-    <row r="19" spans="1:13" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="241" t="s">
         <v>62</v>
       </c>
@@ -19336,7 +19336,7 @@
       <c r="K19" s="228"/>
       <c r="L19" s="228"/>
     </row>
-    <row r="20" spans="1:13" ht="57.1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" ht="57.2" x14ac:dyDescent="0.25">
       <c r="B20" s="233" t="s">
         <v>67</v>
       </c>
@@ -19365,7 +19365,7 @@
       </c>
       <c r="L20" s="228"/>
     </row>
-    <row r="21" spans="1:13" ht="86.3" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" ht="86.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="241"/>
       <c r="C21" s="209"/>
       <c r="D21" s="209" t="s">
@@ -19384,7 +19384,7 @@
       <c r="K21" s="228"/>
       <c r="L21" s="228"/>
     </row>
-    <row r="22" spans="1:13" ht="47.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" ht="47.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="233" t="s">
         <v>70</v>
       </c>
@@ -19457,7 +19457,7 @@
       <c r="K24" s="228"/>
       <c r="L24" s="228"/>
     </row>
-    <row r="25" spans="1:13" ht="50.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="233" t="s">
         <v>74</v>
       </c>
@@ -19482,7 +19482,7 @@
       <c r="K25" s="228"/>
       <c r="L25" s="228"/>
     </row>
-    <row r="26" spans="1:13" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="241"/>
       <c r="C26" s="248"/>
       <c r="D26" s="248" t="s">
@@ -19501,7 +19501,7 @@
       <c r="K26" s="228"/>
       <c r="L26" s="228"/>
     </row>
-    <row r="27" spans="1:13" ht="199.7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" ht="210" x14ac:dyDescent="0.25">
       <c r="A27" s="311"/>
       <c r="B27" s="233" t="s">
         <v>82</v>
@@ -19538,7 +19538,7 @@
         <v>1601</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="241"/>
       <c r="C28" s="209"/>
       <c r="D28" s="209" t="s">
@@ -19553,7 +19553,7 @@
       <c r="K28" s="228"/>
       <c r="L28" s="228"/>
     </row>
-    <row r="29" spans="1:13" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="241" t="s">
         <v>1626</v>
       </c>
@@ -19574,7 +19574,7 @@
       <c r="K29" s="228"/>
       <c r="L29" s="228"/>
     </row>
-    <row r="30" spans="1:13" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="241" t="s">
         <v>203</v>
       </c>
@@ -19595,7 +19595,7 @@
       <c r="K30" s="228"/>
       <c r="L30" s="228"/>
     </row>
-    <row r="31" spans="1:13" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="241" t="s">
         <v>204</v>
       </c>
@@ -19616,7 +19616,7 @@
       <c r="K31" s="228"/>
       <c r="L31" s="228"/>
     </row>
-    <row r="32" spans="1:13" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="241" t="s">
         <v>1201</v>
       </c>
@@ -19635,7 +19635,7 @@
       <c r="K32" s="228"/>
       <c r="L32" s="228"/>
     </row>
-    <row r="33" spans="1:12" s="172" customFormat="1" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" s="172" customFormat="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="208"/>
       <c r="B33" s="251" t="s">
         <v>1324</v>
@@ -19661,7 +19661,7 @@
       </c>
       <c r="L33" s="255"/>
     </row>
-    <row r="34" spans="1:12" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
       <c r="B34" s="233" t="s">
         <v>101</v>
       </c>
@@ -19690,7 +19690,7 @@
       <c r="K34" s="228"/>
       <c r="L34" s="228"/>
     </row>
-    <row r="35" spans="1:12" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B35" s="241"/>
       <c r="C35" s="209"/>
       <c r="D35" s="209" t="s">
@@ -19707,7 +19707,7 @@
       <c r="K35" s="228"/>
       <c r="L35" s="228"/>
     </row>
-    <row r="36" spans="1:12" ht="100.55" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" ht="100.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="233" t="s">
         <v>102</v>
       </c>
@@ -19730,7 +19730,7 @@
       <c r="K36" s="228"/>
       <c r="L36" s="228"/>
     </row>
-    <row r="37" spans="1:12" ht="99.85" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" ht="99.95" x14ac:dyDescent="0.25">
       <c r="B37" s="237"/>
       <c r="C37" s="177"/>
       <c r="D37" s="177" t="s">
@@ -19749,7 +19749,7 @@
       <c r="K37" s="228"/>
       <c r="L37" s="228"/>
     </row>
-    <row r="38" spans="1:12" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B38" s="241"/>
       <c r="C38" s="209"/>
       <c r="D38" s="209" t="s">
@@ -19867,7 +19867,7 @@
       <c r="K42" s="228"/>
       <c r="L42" s="228"/>
     </row>
-    <row r="43" spans="1:12" ht="72" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B43" s="257" t="s">
         <v>240</v>
       </c>
@@ -19896,7 +19896,7 @@
       <c r="K43" s="228"/>
       <c r="L43" s="228"/>
     </row>
-    <row r="44" spans="1:12" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B44" s="257" t="s">
         <v>8</v>
       </c>
@@ -19927,7 +19927,7 @@
       </c>
       <c r="L44" s="228"/>
     </row>
-    <row r="45" spans="1:12" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B45" s="257" t="s">
         <v>1715</v>
       </c>
@@ -19958,7 +19958,7 @@
       </c>
       <c r="L45" s="228"/>
     </row>
-    <row r="46" spans="1:12" ht="57.1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="B46" s="233" t="s">
         <v>193</v>
       </c>
@@ -20008,7 +20008,7 @@
       <c r="K47" s="228"/>
       <c r="L47" s="228"/>
     </row>
-    <row r="48" spans="1:12" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B48" s="241" t="s">
         <v>1020</v>
       </c>
@@ -20077,7 +20077,7 @@
       <c r="K50" s="228"/>
       <c r="L50" s="228"/>
     </row>
-    <row r="51" spans="2:12" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:12" ht="28.5" x14ac:dyDescent="0.25">
       <c r="B51" s="237"/>
       <c r="C51" s="177"/>
       <c r="D51" s="177" t="s">
@@ -20096,7 +20096,7 @@
       <c r="K51" s="228"/>
       <c r="L51" s="228"/>
     </row>
-    <row r="52" spans="2:12" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:12" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B52" s="241"/>
       <c r="C52" s="209"/>
       <c r="D52" s="209" t="s">
@@ -20165,7 +20165,7 @@
       <c r="K54" s="228"/>
       <c r="L54" s="228"/>
     </row>
-    <row r="55" spans="2:12" ht="57.1" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:12" ht="75" x14ac:dyDescent="0.25">
       <c r="B55" s="233" t="s">
         <v>210</v>
       </c>
@@ -20194,7 +20194,7 @@
       <c r="K55" s="228"/>
       <c r="L55" s="228"/>
     </row>
-    <row r="56" spans="2:12" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:12" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B56" s="270"/>
       <c r="C56" s="209"/>
       <c r="D56" s="209" t="s">
@@ -20244,7 +20244,7 @@
       </c>
       <c r="L57" s="228"/>
     </row>
-    <row r="58" spans="2:12" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B58" s="257" t="s">
         <v>123</v>
       </c>
@@ -20337,7 +20337,7 @@
       </c>
       <c r="L60" s="228"/>
     </row>
-    <row r="61" spans="2:12" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:12" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B61" s="241" t="s">
         <v>1761</v>
       </c>
@@ -20435,7 +20435,7 @@
       <c r="K64" s="228"/>
       <c r="L64" s="228"/>
     </row>
-    <row r="65" spans="1:12" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B65" s="241" t="s">
         <v>957</v>
       </c>
@@ -20462,7 +20462,7 @@
       <c r="K65" s="228"/>
       <c r="L65" s="228"/>
     </row>
-    <row r="66" spans="1:12" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B66" s="241" t="s">
         <v>958</v>
       </c>
@@ -20489,7 +20489,7 @@
       <c r="K66" s="228"/>
       <c r="L66" s="228"/>
     </row>
-    <row r="67" spans="1:12" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B67" s="241" t="s">
         <v>959</v>
       </c>
@@ -20516,7 +20516,7 @@
       <c r="K67" s="228"/>
       <c r="L67" s="228"/>
     </row>
-    <row r="68" spans="1:12" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B68" s="241" t="s">
         <v>961</v>
       </c>
@@ -20543,7 +20543,7 @@
       <c r="K68" s="228"/>
       <c r="L68" s="228"/>
     </row>
-    <row r="69" spans="1:12" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B69" s="241" t="s">
         <v>962</v>
       </c>
@@ -20570,7 +20570,7 @@
       <c r="K69" s="228"/>
       <c r="L69" s="228"/>
     </row>
-    <row r="70" spans="1:12" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B70" s="241" t="s">
         <v>963</v>
       </c>
@@ -20647,7 +20647,7 @@
       <c r="K72" s="228"/>
       <c r="L72" s="228"/>
     </row>
-    <row r="73" spans="1:12" ht="68.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" ht="68.650000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="207"/>
       <c r="B73" s="233" t="s">
         <v>917</v>
@@ -20677,7 +20677,7 @@
       <c r="K73" s="228"/>
       <c r="L73" s="228"/>
     </row>
-    <row r="74" spans="1:12" s="11" customFormat="1" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" s="11" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A74" s="207"/>
       <c r="B74" s="276" t="s">
         <v>275</v>
@@ -20720,7 +20720,7 @@
       <c r="K75" s="228"/>
       <c r="L75" s="228"/>
     </row>
-    <row r="76" spans="1:12" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B76" s="241" t="s">
         <v>1288</v>
       </c>
@@ -20764,7 +20764,7 @@
       <c r="K77" s="228"/>
       <c r="L77" s="228"/>
     </row>
-    <row r="78" spans="1:12" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B78" s="241" t="s">
         <v>277</v>
       </c>
@@ -20848,7 +20848,7 @@
       <c r="K81" s="228"/>
       <c r="L81" s="228"/>
     </row>
-    <row r="82" spans="2:12" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:12" ht="45" x14ac:dyDescent="0.25">
       <c r="B82" s="265" t="s">
         <v>294</v>
       </c>
@@ -20900,7 +20900,7 @@
       <c r="K83" s="228"/>
       <c r="L83" s="228"/>
     </row>
-    <row r="84" spans="2:12" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B84" s="241" t="s">
         <v>1190</v>
       </c>
@@ -20923,7 +20923,7 @@
       <c r="K84" s="228"/>
       <c r="L84" s="228"/>
     </row>
-    <row r="85" spans="2:12" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B85" s="241" t="s">
         <v>327</v>
       </c>
@@ -20965,7 +20965,7 @@
       <c r="K86" s="228"/>
       <c r="L86" s="228"/>
     </row>
-    <row r="87" spans="2:12" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:12" ht="28.5" x14ac:dyDescent="0.25">
       <c r="B87" s="233" t="s">
         <v>337</v>
       </c>
@@ -20994,7 +20994,7 @@
       <c r="K87" s="228"/>
       <c r="L87" s="228"/>
     </row>
-    <row r="88" spans="2:12" ht="42.8" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:12" ht="45" x14ac:dyDescent="0.25">
       <c r="B88" s="237" t="s">
         <v>341</v>
       </c>
@@ -21023,7 +21023,7 @@
       <c r="K88" s="228"/>
       <c r="L88" s="228"/>
     </row>
-    <row r="89" spans="2:12" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B89" s="283" t="s">
         <v>345</v>
       </c>
@@ -21052,7 +21052,7 @@
       <c r="K89" s="228"/>
       <c r="L89" s="228"/>
     </row>
-    <row r="90" spans="2:12" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:12" ht="28.5" x14ac:dyDescent="0.25">
       <c r="B90" s="287" t="s">
         <v>968</v>
       </c>
@@ -21115,7 +21115,7 @@
       <c r="K92" s="228"/>
       <c r="L92" s="228"/>
     </row>
-    <row r="93" spans="2:12" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B93" s="289" t="s">
         <v>1079</v>
       </c>
@@ -21136,7 +21136,7 @@
       <c r="K93" s="228"/>
       <c r="L93" s="228"/>
     </row>
-    <row r="94" spans="2:12" ht="42.8" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:12" ht="45" x14ac:dyDescent="0.25">
       <c r="B94" s="292" t="s">
         <v>1101</v>
       </c>
@@ -21165,7 +21165,7 @@
       <c r="K94" s="228"/>
       <c r="L94" s="228"/>
     </row>
-    <row r="95" spans="2:12" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="2:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B95" s="289" t="s">
         <v>1080</v>
       </c>
@@ -21203,7 +21203,7 @@
       <c r="K96" s="228"/>
       <c r="L96" s="228"/>
     </row>
-    <row r="97" spans="1:12" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B97" s="289" t="s">
         <v>1093</v>
       </c>
@@ -21245,7 +21245,7 @@
       <c r="K98" s="296"/>
       <c r="L98" s="297"/>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:12" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B99" s="298" t="s">
         <v>1081</v>
       </c>
@@ -21266,7 +21266,7 @@
       <c r="K99" s="296"/>
       <c r="L99" s="297"/>
     </row>
-    <row r="100" spans="1:12" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B100" s="287" t="s">
         <v>1107</v>
       </c>
@@ -21287,7 +21287,7 @@
       <c r="K100" s="296"/>
       <c r="L100" s="297"/>
     </row>
-    <row r="101" spans="1:12" ht="42.8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:12" ht="42.75" x14ac:dyDescent="0.25">
       <c r="B101" s="299" t="s">
         <v>1111</v>
       </c>
@@ -21316,7 +21316,7 @@
       <c r="K101" s="296"/>
       <c r="L101" s="297"/>
     </row>
-    <row r="102" spans="1:12" ht="42.8" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A102" s="173"/>
       <c r="B102" s="287" t="s">
         <v>1191</v>
@@ -21342,7 +21342,7 @@
       <c r="K102" s="301"/>
       <c r="L102" s="302"/>
     </row>
-    <row r="103" spans="1:12" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" s="173"/>
       <c r="B103" s="291" t="s">
         <v>1313</v>
@@ -21362,7 +21362,7 @@
       <c r="K103" s="249"/>
       <c r="L103" s="250"/>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:12" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B104" s="256" t="s">
         <v>1386</v>
       </c>
@@ -21383,7 +21383,7 @@
       <c r="K104" s="303"/>
       <c r="L104" s="303"/>
     </row>
-    <row r="105" spans="1:12" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B105" s="178" t="s">
         <v>1388</v>
       </c>
@@ -21404,7 +21404,7 @@
       <c r="K105" s="304"/>
       <c r="L105" s="304"/>
     </row>
-    <row r="106" spans="1:12" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
       <c r="B106" s="178" t="s">
         <v>1389</v>
       </c>
@@ -21425,7 +21425,7 @@
       <c r="K106" s="304"/>
       <c r="L106" s="304"/>
     </row>
-    <row r="107" spans="1:12" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
       <c r="B107" s="178" t="s">
         <v>1390</v>
       </c>
@@ -21446,7 +21446,7 @@
       <c r="K107" s="304"/>
       <c r="L107" s="304"/>
     </row>
-    <row r="108" spans="1:12" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
       <c r="B108" s="178" t="s">
         <v>1391</v>
       </c>
@@ -21467,7 +21467,7 @@
       <c r="K108" s="304"/>
       <c r="L108" s="304"/>
     </row>
-    <row r="109" spans="1:12" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
       <c r="B109" s="178" t="s">
         <v>1392</v>
       </c>
@@ -21488,7 +21488,7 @@
       <c r="K109" s="304"/>
       <c r="L109" s="304"/>
     </row>
-    <row r="110" spans="1:12" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
       <c r="B110" s="178" t="s">
         <v>960</v>
       </c>
@@ -21509,7 +21509,7 @@
       <c r="K110" s="304"/>
       <c r="L110" s="304"/>
     </row>
-    <row r="111" spans="1:12" ht="42.8" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="B111" s="306" t="s">
         <v>1605</v>
       </c>
@@ -21532,7 +21532,7 @@
       <c r="K111" s="304"/>
       <c r="L111" s="304"/>
     </row>
-    <row r="112" spans="1:12" ht="42.8" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:12" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A112" s="60"/>
       <c r="B112" s="178" t="s">
         <v>1666</v>
@@ -21556,7 +21556,7 @@
       <c r="K112" s="304"/>
       <c r="L112" s="304"/>
     </row>
-    <row r="113" spans="1:12" ht="42.8" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:12" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A113" s="60"/>
       <c r="B113" s="6" t="s">
         <v>1735</v>
@@ -21576,7 +21576,7 @@
       <c r="K113" s="307"/>
       <c r="L113" s="307"/>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:12" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A114" s="60"/>
     </row>
     <row r="119" spans="1:12" x14ac:dyDescent="0.25">
@@ -21589,7 +21589,7 @@
         <v>1728</v>
       </c>
     </row>
-    <row r="121" spans="1:12" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:12" ht="28.5" x14ac:dyDescent="0.25">
       <c r="B121" s="6" t="s">
         <v>1735</v>
       </c>
@@ -21612,7 +21612,7 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -22652,7 +22652,7 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
@@ -22734,19 +22734,19 @@
       <selection activeCell="F381" sqref="F381"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="6.625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="2.5703125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="6.5703125" style="3" customWidth="1"/>
     <col min="3" max="3" width="68" style="3" customWidth="1"/>
-    <col min="4" max="4" width="24.5" style="3" customWidth="1"/>
-    <col min="5" max="5" width="21.375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="15.5" style="3" customWidth="1"/>
-    <col min="7" max="7" width="19.125" style="3" customWidth="1"/>
-    <col min="8" max="16384" width="11.5" style="3"/>
+    <col min="4" max="4" width="24.42578125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="21.42578125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" style="3" customWidth="1"/>
+    <col min="8" max="16384" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="9.5500000000000007" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1" spans="2:7" ht="9.6" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C2" s="3" t="s">
         <v>973</v>
@@ -22761,7 +22761,7 @@
       </c>
     </row>
     <row r="3" spans="2:7" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="2:7" ht="42.8" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B4" s="48" t="s">
         <v>22</v>
       </c>
@@ -22803,7 +22803,7 @@
         <v>60.383771352525045</v>
       </c>
     </row>
-    <row r="6" spans="2:7" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B6" s="31">
         <v>49</v>
       </c>
@@ -22847,7 +22847,7 @@
         <v>44.913600688428012</v>
       </c>
     </row>
-    <row r="8" spans="2:7" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B8" s="31">
         <v>318</v>
       </c>
@@ -22891,7 +22891,7 @@
         <v>22.765397003308141</v>
       </c>
     </row>
-    <row r="10" spans="2:7" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="31">
         <v>35</v>
       </c>
@@ -23111,7 +23111,7 @@
         <v>13.577132508214365</v>
       </c>
     </row>
-    <row r="20" spans="2:7" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B20" s="31">
         <v>33</v>
       </c>
@@ -23243,7 +23243,7 @@
         <v>9.2747730630265064</v>
       </c>
     </row>
-    <row r="26" spans="2:7" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B26" s="31">
         <v>26</v>
       </c>
@@ -23353,7 +23353,7 @@
         <v>7.9716739069776867</v>
       </c>
     </row>
-    <row r="31" spans="2:7" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B31" s="31">
         <v>121</v>
       </c>
@@ -23639,7 +23639,7 @@
         <v>5.6058870246207277</v>
       </c>
     </row>
-    <row r="44" spans="2:7" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B44" s="31">
         <v>357</v>
       </c>
@@ -23661,7 +23661,7 @@
         <v>5.5413928274990685</v>
       </c>
     </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B45" s="31">
         <v>2</v>
       </c>
@@ -23793,7 +23793,7 @@
         <v>5.0227698432867252</v>
       </c>
     </row>
-    <row r="51" spans="2:7" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B51" s="31">
         <v>325</v>
       </c>
@@ -24057,7 +24057,7 @@
         <v>4.4056094807433848</v>
       </c>
     </row>
-    <row r="63" spans="2:7" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B63" s="31">
         <v>331</v>
       </c>
@@ -24299,7 +24299,7 @@
         <v>3.8836909320383666</v>
       </c>
     </row>
-    <row r="74" spans="2:7" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B74" s="31">
         <v>168</v>
       </c>
@@ -24695,7 +24695,7 @@
         <v>2.7174236137254351</v>
       </c>
     </row>
-    <row r="92" spans="2:7" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B92" s="31">
         <v>322</v>
       </c>
@@ -24849,7 +24849,7 @@
         <v>2.4234922166237074</v>
       </c>
     </row>
-    <row r="99" spans="2:7" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B99" s="31">
         <v>358</v>
       </c>
@@ -24893,7 +24893,7 @@
         <v>2.4018733135517563</v>
       </c>
     </row>
-    <row r="101" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B101" s="31">
         <v>93</v>
       </c>
@@ -25157,7 +25157,7 @@
         <v>2.0240698001114366</v>
       </c>
     </row>
-    <row r="113" spans="2:7" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B113" s="31">
         <v>226</v>
       </c>
@@ -25355,7 +25355,7 @@
         <v>1.877581958412011</v>
       </c>
     </row>
-    <row r="122" spans="2:7" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B122" s="31">
         <v>43</v>
       </c>
@@ -25399,7 +25399,7 @@
         <v>1.8606098012747323</v>
       </c>
     </row>
-    <row r="124" spans="2:7" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B124" s="31">
         <v>39</v>
       </c>
@@ -25421,7 +25421,7 @@
         <v>1.7908427009647918</v>
       </c>
     </row>
-    <row r="125" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B125" s="31">
         <v>83</v>
       </c>
@@ -25597,7 +25597,7 @@
         <v>1.682319762220988</v>
       </c>
     </row>
-    <row r="133" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B133" s="31">
         <v>101</v>
       </c>
@@ -25773,7 +25773,7 @@
         <v>1.5817720895494585</v>
       </c>
     </row>
-    <row r="141" spans="2:7" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B141" s="31">
         <v>199</v>
       </c>
@@ -25883,7 +25883,7 @@
         <v>1.4186086915170946</v>
       </c>
     </row>
-    <row r="146" spans="2:7" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B146" s="31">
         <v>202</v>
       </c>
@@ -25927,7 +25927,7 @@
         <v>1.3961988529669012</v>
       </c>
     </row>
-    <row r="148" spans="2:7" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B148" s="31">
         <v>234</v>
       </c>
@@ -26103,7 +26103,7 @@
         <v>1.2597954386150623</v>
       </c>
     </row>
-    <row r="156" spans="2:7" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="156" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B156" s="31">
         <v>34</v>
       </c>
@@ -26147,7 +26147,7 @@
         <v>1.2335627452533655</v>
       </c>
     </row>
-    <row r="158" spans="2:7" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="158" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B158" s="31">
         <v>204</v>
       </c>
@@ -26235,7 +26235,7 @@
         <v>1.1546998869436407</v>
       </c>
     </row>
-    <row r="162" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="162" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B162" s="31">
         <v>124</v>
       </c>
@@ -26433,7 +26433,7 @@
         <v>1.0582057585981022</v>
       </c>
     </row>
-    <row r="171" spans="2:7" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="171" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B171" s="31">
         <v>344</v>
       </c>
@@ -26543,7 +26543,7 @@
         <v>1.0059051500993421</v>
       </c>
     </row>
-    <row r="176" spans="2:7" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="176" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B176" s="31">
         <v>238</v>
       </c>
@@ -26631,7 +26631,7 @@
         <v>0.96803911407850063</v>
       </c>
     </row>
-    <row r="180" spans="2:7" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="180" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B180" s="31">
         <v>198</v>
       </c>
@@ -27027,7 +27027,7 @@
         <v>0.79884483302454057</v>
       </c>
     </row>
-    <row r="198" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="198" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B198" s="31">
         <v>255</v>
       </c>
@@ -27049,7 +27049,7 @@
         <v>0.79759251851732393</v>
       </c>
     </row>
-    <row r="199" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="199" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B199" s="31">
         <v>206</v>
       </c>
@@ -27159,7 +27159,7 @@
         <v>0.66478126946250127</v>
       </c>
     </row>
-    <row r="204" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="204" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B204" s="31">
         <v>321</v>
       </c>
@@ -27335,7 +27335,7 @@
         <v>0.563146060508389</v>
       </c>
     </row>
-    <row r="212" spans="2:7" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="212" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B212" s="31">
         <v>236</v>
       </c>
@@ -27379,7 +27379,7 @@
         <v>0.56070734278380907</v>
       </c>
     </row>
-    <row r="214" spans="2:7" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="214" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B214" s="31">
         <v>352</v>
       </c>
@@ -27577,7 +27577,7 @@
         <v>0.46404843621363678</v>
       </c>
     </row>
-    <row r="223" spans="2:7" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="223" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B223" s="31">
         <v>257</v>
       </c>
@@ -27797,7 +27797,7 @@
         <v>0.39615980766452152</v>
       </c>
     </row>
-    <row r="233" spans="2:7" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="233" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B233" s="31">
         <v>108</v>
       </c>
@@ -27951,7 +27951,7 @@
         <v>0.34194777176000962</v>
       </c>
     </row>
-    <row r="240" spans="2:7" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="240" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B240" s="31">
         <v>233</v>
       </c>
@@ -27995,7 +27995,7 @@
         <v>0.33443388471670948</v>
       </c>
     </row>
-    <row r="242" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="242" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B242" s="31">
         <v>116</v>
       </c>
@@ -28017,7 +28017,7 @@
         <v>0.31123311068827397</v>
       </c>
     </row>
-    <row r="243" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="243" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B243" s="31">
         <v>112</v>
       </c>
@@ -28105,7 +28105,7 @@
         <v>0.30553178411594534</v>
       </c>
     </row>
-    <row r="247" spans="2:7" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="247" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B247" s="31">
         <v>341</v>
       </c>
@@ -28149,7 +28149,7 @@
         <v>0.27646490529054746</v>
       </c>
     </row>
-    <row r="249" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="249" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B249" s="31">
         <v>280</v>
       </c>
@@ -28303,7 +28303,7 @@
         <v>0.23082133706699184</v>
       </c>
     </row>
-    <row r="256" spans="2:7" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="256" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B256" s="31">
         <v>253</v>
       </c>
@@ -28325,7 +28325,7 @@
         <v>0.22633936935695317</v>
       </c>
     </row>
-    <row r="257" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="257" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B257" s="31">
         <v>88</v>
       </c>
@@ -28413,7 +28413,7 @@
         <v>0.20824672029216468</v>
       </c>
     </row>
-    <row r="261" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="261" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B261" s="31">
         <v>258</v>
       </c>
@@ -28523,7 +28523,7 @@
         <v>0.18016851081456944</v>
       </c>
     </row>
-    <row r="266" spans="2:7" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="266" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B266" s="31">
         <v>263</v>
       </c>
@@ -28633,7 +28633,7 @@
         <v>0.13534883371418269</v>
       </c>
     </row>
-    <row r="271" spans="2:7" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="271" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B271" s="31">
         <v>71</v>
       </c>
@@ -28721,7 +28721,7 @@
         <v>9.3956543686178437E-2</v>
       </c>
     </row>
-    <row r="275" spans="2:7" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="275" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B275" s="31">
         <v>270</v>
       </c>
@@ -28853,7 +28853,7 @@
         <v>6.7262471295506901E-2</v>
       </c>
     </row>
-    <row r="281" spans="2:7" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="281" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B281" s="31">
         <v>254</v>
       </c>
@@ -28963,7 +28963,7 @@
         <v>5.1048293991543453E-2</v>
       </c>
     </row>
-    <row r="286" spans="2:7" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="286" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B286" s="31">
         <v>139</v>
       </c>
@@ -29117,7 +29117,7 @@
         <v>-9.260536224418147E-3</v>
       </c>
     </row>
-    <row r="293" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="293" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B293" s="31">
         <v>38</v>
       </c>
@@ -29205,7 +29205,7 @@
         <v>-3.87887940787906E-2</v>
       </c>
     </row>
-    <row r="297" spans="2:7" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="297" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B297" s="31">
         <v>297</v>
       </c>
@@ -29293,7 +29293,7 @@
         <v>-5.8331491520356299E-2</v>
       </c>
     </row>
-    <row r="301" spans="2:7" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="301" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B301" s="31">
         <v>42</v>
       </c>
@@ -29557,7 +29557,7 @@
         <v>-0.13238282567077472</v>
       </c>
     </row>
-    <row r="313" spans="2:7" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="313" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B313" s="31">
         <v>41</v>
       </c>
@@ -29579,7 +29579,7 @@
         <v>-0.13445903130116027</v>
       </c>
     </row>
-    <row r="314" spans="2:7" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="314" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B314" s="31">
         <v>286</v>
       </c>
@@ -29821,7 +29821,7 @@
         <v>-0.23151340561045369</v>
       </c>
     </row>
-    <row r="325" spans="2:7" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="325" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B325" s="31">
         <v>174</v>
       </c>
@@ -29843,7 +29843,7 @@
         <v>-0.23398507897996032</v>
       </c>
     </row>
-    <row r="326" spans="2:7" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="326" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B326" s="31">
         <v>40</v>
       </c>
@@ -30019,7 +30019,7 @@
         <v>-0.34138752579625475</v>
       </c>
     </row>
-    <row r="334" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="334" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B334" s="31">
         <v>261</v>
       </c>
@@ -30041,7 +30041,7 @@
         <v>-0.34425466690488243</v>
       </c>
     </row>
-    <row r="335" spans="2:7" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="335" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B335" s="31">
         <v>45</v>
       </c>
@@ -30239,7 +30239,7 @@
         <v>-0.47334192808298164</v>
       </c>
     </row>
-    <row r="344" spans="2:7" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="344" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B344" s="31">
         <v>304</v>
       </c>
@@ -30745,7 +30745,7 @@
         <v>-8.0795047771780304</v>
       </c>
     </row>
-    <row r="367" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="367" spans="2:7" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B367" s="52"/>
     </row>
     <row r="368" spans="2:7" x14ac:dyDescent="0.25">
@@ -30767,15 +30767,15 @@
       </c>
       <c r="G368" s="41"/>
     </row>
-    <row r="369" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="369" spans="2:7" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B369" s="53"/>
     </row>
-    <row r="377" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="377" spans="2:7" ht="14.25" x14ac:dyDescent="0.25">
       <c r="D377" s="305" t="s">
         <v>1670</v>
       </c>
     </row>
-    <row r="380" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="380" spans="2:7" ht="14.25" x14ac:dyDescent="0.25">
       <c r="E380" s="3">
         <v>100</v>
       </c>
@@ -30783,7 +30783,7 @@
         <v>1671</v>
       </c>
     </row>
-    <row r="381" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="381" spans="2:7" ht="14.25" x14ac:dyDescent="0.25">
       <c r="E381" s="3">
         <v>10000</v>
       </c>
@@ -30796,13 +30796,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="382" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="382" spans="2:7" ht="14.25" x14ac:dyDescent="0.25">
       <c r="E382" s="3">
         <f>E380/E381</f>
         <v>0.01</v>
       </c>
     </row>
-    <row r="383" spans="2:7" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="383" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="E383" s="3" t="s">
         <v>1673</v>
       </c>
@@ -30870,13 +30870,13 @@
       <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.5" customWidth="1"/>
-    <col min="8" max="8" width="7.5" customWidth="1"/>
-    <col min="9" max="9" width="10.375" customWidth="1"/>
-    <col min="12" max="12" width="16.375" customWidth="1"/>
-    <col min="13" max="13" width="3.5" customWidth="1"/>
+    <col min="1" max="1" width="1.42578125" customWidth="1"/>
+    <col min="8" max="8" width="7.42578125" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" customWidth="1"/>
+    <col min="12" max="12" width="16.42578125" customWidth="1"/>
+    <col min="13" max="13" width="3.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:14" x14ac:dyDescent="0.25">
@@ -31105,17 +31105,17 @@
       <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.375" customWidth="1"/>
-    <col min="2" max="2" width="14.625" customWidth="1"/>
-    <col min="3" max="3" width="45.875" customWidth="1"/>
-    <col min="4" max="4" width="16.625" customWidth="1"/>
-    <col min="5" max="5" width="11.875" customWidth="1"/>
-    <col min="6" max="6" width="59.375" customWidth="1"/>
+    <col min="1" max="1" width="2.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" customWidth="1"/>
+    <col min="3" max="3" width="45.85546875" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" customWidth="1"/>
+    <col min="6" max="6" width="59.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="C2" s="12" t="s">
         <v>351</v>
       </c>
@@ -31131,7 +31131,7 @@
       <c r="E3" s="12"/>
       <c r="F3" s="12"/>
     </row>
-    <row r="5" spans="2:6" s="1" customFormat="1" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="192" t="s">
         <v>471</v>
       </c>
@@ -31161,7 +31161,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B7" s="195">
         <v>2</v>
       </c>
@@ -31221,7 +31221,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B11" s="195">
         <v>6</v>
       </c>
@@ -31236,7 +31236,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B12" s="195">
         <v>7</v>
       </c>
@@ -31266,7 +31266,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B14" s="195">
         <v>9</v>
       </c>
@@ -31281,7 +31281,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B15" s="195">
         <v>10</v>
       </c>
@@ -31311,7 +31311,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B17" s="195">
         <v>12</v>
       </c>
@@ -31341,7 +31341,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B19" s="195">
         <v>14</v>
       </c>
@@ -31356,7 +31356,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B20" s="195">
         <v>15</v>
       </c>
@@ -31371,7 +31371,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B21" s="195">
         <v>16</v>
       </c>
@@ -31431,7 +31431,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B25" s="195">
         <v>20</v>
       </c>
@@ -31461,7 +31461,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B27" s="195">
         <v>22</v>
       </c>
@@ -31476,7 +31476,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B28" s="195">
         <v>23</v>
       </c>
@@ -31506,7 +31506,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B30" s="195">
         <v>25</v>
       </c>
@@ -31521,7 +31521,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B31" s="195">
         <v>26</v>
       </c>
@@ -31536,7 +31536,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B32" s="195">
         <v>27</v>
       </c>
@@ -31566,7 +31566,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="34" spans="2:6" ht="42.8" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:6" ht="42.75" x14ac:dyDescent="0.25">
       <c r="B34" s="195">
         <v>29</v>
       </c>
@@ -31596,7 +31596,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B36" s="195">
         <v>31</v>
       </c>
@@ -31611,7 +31611,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B37" s="195">
         <v>32</v>
       </c>
@@ -31626,7 +31626,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B38" s="195">
         <v>33</v>
       </c>
@@ -31641,7 +31641,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B39" s="195">
         <v>34</v>
       </c>
@@ -31758,42 +31758,42 @@
         <v>397</v>
       </c>
     </row>
-    <row r="52" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="6:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="F52" s="12" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="53" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="6:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="F53" s="12" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="54" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="6:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="F54" s="12" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="55" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="6:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="F55" s="12" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="56" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="6:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="F56" s="12" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="57" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="6:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="F57" s="12" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="58" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="6:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="F58" s="12" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="59" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="6:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="F59" s="12" t="s">
         <v>405</v>
       </c>
@@ -32047,12 +32047,12 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
     <col min="3" max="3" width="43" style="1" customWidth="1"/>
-    <col min="4" max="4" width="37.5" customWidth="1"/>
+    <col min="4" max="4" width="37.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -32387,21 +32387,21 @@
       <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.75" style="2" customWidth="1"/>
-    <col min="2" max="2" width="16.5" style="2" customWidth="1"/>
-    <col min="3" max="8" width="10.625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="7.5" style="2" customWidth="1"/>
-    <col min="10" max="10" width="9.5" style="2" customWidth="1"/>
-    <col min="11" max="11" width="7.5" style="2" customWidth="1"/>
-    <col min="12" max="13" width="11.5" style="2"/>
-    <col min="14" max="14" width="9.5" style="2" customWidth="1"/>
-    <col min="15" max="15" width="8.625" style="2" customWidth="1"/>
-    <col min="16" max="16384" width="11.5" style="2"/>
+    <col min="1" max="1" width="3.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" style="2" customWidth="1"/>
+    <col min="3" max="8" width="10.5703125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="7.42578125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="9.42578125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="7.42578125" style="2" customWidth="1"/>
+    <col min="12" max="13" width="11.42578125" style="2"/>
+    <col min="14" max="14" width="9.42578125" style="2" customWidth="1"/>
+    <col min="15" max="15" width="8.5703125" style="2" customWidth="1"/>
+    <col min="16" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:11" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
@@ -32421,7 +32421,7 @@
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
     </row>
-    <row r="4" spans="2:11" ht="15.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:11" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="67" t="s">
         <v>481</v>
       </c>
@@ -32437,7 +32437,7 @@
       <c r="J4" s="5"/>
       <c r="K4" s="5"/>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B5" s="68"/>
       <c r="C5" s="326" t="s">
         <v>1135</v>
@@ -32539,7 +32539,7 @@
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:11" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B10" s="86" t="s">
         <v>476</v>
       </c>
@@ -32565,7 +32565,7 @@
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:11" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B11" s="90"/>
       <c r="C11" s="104"/>
       <c r="D11" s="104"/>
@@ -32581,7 +32581,7 @@
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:11" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B12" s="86" t="s">
         <v>477</v>
       </c>
@@ -32607,7 +32607,7 @@
       <c r="J12" s="5"/>
       <c r="K12" s="5"/>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:11" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B13" s="90"/>
       <c r="C13" s="104"/>
       <c r="D13" s="104"/>
@@ -32623,7 +32623,7 @@
       <c r="J13" s="5"/>
       <c r="K13" s="5"/>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:11" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B14" s="86" t="s">
         <v>478</v>
       </c>
@@ -32649,7 +32649,7 @@
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:11" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B15" s="90"/>
       <c r="C15" s="104"/>
       <c r="D15" s="104"/>
@@ -32665,7 +32665,7 @@
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:11" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B16" s="67" t="s">
         <v>479</v>
       </c>
@@ -32691,7 +32691,7 @@
       <c r="J16" s="5"/>
       <c r="K16" s="5"/>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:11" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B17" s="90"/>
       <c r="C17" s="104"/>
       <c r="D17" s="104"/>
@@ -32707,7 +32707,7 @@
       <c r="J17" s="5"/>
       <c r="K17" s="5"/>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:11" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B18" s="111" t="s">
         <v>480</v>
       </c>
@@ -32733,7 +32733,7 @@
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:11" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B19" s="99"/>
       <c r="C19" s="106"/>
       <c r="D19" s="106"/>
@@ -32749,7 +32749,7 @@
       <c r="J19" s="5"/>
       <c r="K19" s="5"/>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:11" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>

</xml_diff>